<commit_message>
push after graph changed color
</commit_message>
<xml_diff>
--- a/Graph/BFD_Summary.xlsx
+++ b/Graph/BFD_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POLITO\Architetture Dei Sistemi Di Elaborazione\Progetto Speciale\Reti Neurali\posit-nn-fault-injection\Graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1E2CDF-A954-42B2-9629-A55F8557E593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000EDCC2-95BE-47C1-A611-43A398CD1085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="798" xr2:uid="{08A9326E-C172-4056-BC64-C4AC58E1DE07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="798" xr2:uid="{08A9326E-C172-4056-BC64-C4AC58E1DE07}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -741,6 +741,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF75E6DA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -773,29 +778,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>LAYER 0</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Livello convolutivo 0</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -812,19 +810,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -847,19 +839,13 @@
             <c:v>Posit 32</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -914,19 +900,13 @@
             <c:v>Float 32</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -964,6 +944,21 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
         <c:smooth val="0"/>
         <c:axId val="456196208"/>
         <c:axId val="456198128"/>
@@ -982,10 +977,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1013,10 +1009,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1036,9 +1033,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="10000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1046,14 +1043,15 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1079,20 +1077,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1100,10 +1084,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1131,10 +1116,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1162,10 +1148,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1181,7 +1168,19 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1205,8 +1204,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1230,28 +1230,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:srgbClr val="75E6DA"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1294,19 +1283,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -1314,13 +1297,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>LAYER</a:t>
+              <a:t>Livello convolutivo 1</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" baseline="0"/>
-              <a:t> 1</a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1337,19 +1315,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -1372,19 +1344,13 @@
             <c:v>Posit 32</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1439,19 +1405,13 @@
             <c:v>Float 32</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -1489,6 +1449,21 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
         <c:smooth val="0"/>
         <c:axId val="487925632"/>
         <c:axId val="487926112"/>
@@ -1507,10 +1482,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1538,10 +1514,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1561,9 +1538,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="10000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1575,10 +1552,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1604,20 +1582,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1625,10 +1589,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -1656,10 +1621,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -1687,10 +1653,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1706,7 +1673,19 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1730,8 +1709,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1755,28 +1735,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:srgbClr val="75E6DA"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1879,41 +1848,43 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1921,36 +1892,29 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1969,6 +1933,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1976,36 +1948,60 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2017,15 +2013,18 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2033,15 +2032,15 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2057,16 +2056,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2078,7 +2078,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2089,9 +2089,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2102,17 +2102,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2121,16 +2122,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2139,7 +2140,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -2147,17 +2148,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -2166,14 +2166,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2184,17 +2184,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2203,14 +2202,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2221,8 +2220,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2232,15 +2232,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
   </cs:plotArea>
   <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2248,16 +2263,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2270,17 +2286,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2289,19 +2305,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2310,10 +2319,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2325,8 +2334,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2336,7 +2346,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2344,9 +2354,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2357,59 +2367,62 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea>
+  <cs:chartArea mods="allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2417,36 +2430,29 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2465,6 +2471,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2472,36 +2486,60 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2513,15 +2551,18 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2529,15 +2570,15 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2553,16 +2594,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2574,7 +2616,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2585,9 +2627,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2598,17 +2640,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2617,16 +2660,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2635,7 +2678,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -2643,17 +2686,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -2662,14 +2704,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2680,17 +2722,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2699,14 +2740,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2717,8 +2758,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2728,15 +2770,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
   </cs:plotArea>
   <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2744,16 +2801,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2766,17 +2824,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2785,19 +2843,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2806,10 +2857,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2821,8 +2872,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2832,7 +2884,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2840,9 +2892,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2853,18 +2905,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -2874,15 +2927,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2910,16 +2963,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>5587</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60712</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3631,7 +3684,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>